<commit_message>
Results for ac and btheta
</commit_message>
<xml_diff>
--- a/Results/BTheta_results_case_ieee123_modified_python.xlsx
+++ b/Results/BTheta_results_case_ieee123_modified_python.xlsx
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>-1.500761864047708</v>
+        <v>-1.500761864047709</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>-1.546373543740256</v>
+        <v>-1.546373543740257</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -702,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>-1.60456775533898</v>
+        <v>-1.604567755338981</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>-1.606533776017358</v>
+        <v>-1.606533776017359</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>-1.614791061674796</v>
+        <v>-1.614791061674797</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>-1.632092043919548</v>
+        <v>-1.632092043919549</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>-1.642708555376528</v>
+        <v>-1.642708555376529</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>-1.426888638063171</v>
+        <v>-1.426888638063172</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +1115,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>1.489999999999996</v>
+        <v>1.489999999999995</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>29.99999999999992</v>
+        <v>29.99999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>29.99999999999993</v>
+        <v>29.99999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1169,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>29.99999999999994</v>
+        <v>29.99999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1177,7 +1177,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1185,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>29.99999999999996</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1193,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>29.99999999999997</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1201,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>29.99999999999997</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>29.99999999999997</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>29.99999999999997</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>29.99999999999998</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1281,7 +1281,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1289,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1297,7 +1297,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1321,7 +1321,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1329,7 +1329,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1337,7 +1337,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1345,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1353,7 +1353,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1457,7 +1457,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>30</v>
+        <v>30.00000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1465,7 +1465,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1473,7 +1473,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1481,7 +1481,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1497,7 +1497,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1505,7 +1505,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1513,7 +1513,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1521,7 +1521,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1529,7 +1529,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1537,7 +1537,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1545,7 +1545,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1553,7 +1553,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1561,7 +1561,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1569,7 +1569,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1577,7 +1577,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1585,7 +1585,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>29.99999999999995</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1824,7 +1824,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>-1.119999999999996</v>
+        <v>-1.119999999999998</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1841,7 +1841,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>-1.159999999999995</v>
+        <v>-1.159999999999998</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1875,7 +1875,7 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>-1.274999999999996</v>
+        <v>-1.274999999999995</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1909,7 +1909,7 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>1.424999999999999</v>
+        <v>1.425000000000001</v>
       </c>
       <c r="E18">
         <v>2</v>

</xml_diff>